<commit_message>
Optimising download in one function
</commit_message>
<xml_diff>
--- a/downloads/remains.xlsx
+++ b/downloads/remains.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Караганда_Список_Остатков" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Астана_Список_Остатков" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
   <si>
     <t>МСП</t>
   </si>
@@ -64,12 +64,15 @@
     <t>4/28/1905</t>
   </si>
   <si>
-    <t>Караганда</t>
+    <t>Астана</t>
   </si>
   <si>
     <t>Антикамен (почки) капс №60</t>
   </si>
   <si>
+    <t>М,К</t>
+  </si>
+  <si>
     <t>Беррилакт саше №30 (лактобактерии, манноза, экстр.клюквы)</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">Бонеост (Ибандронат ) Таб покр пленоч оболоч 150 мг, №1  </t>
   </si>
   <si>
+    <t>Назгуль</t>
+  </si>
+  <si>
     <t>Волкрон (Тадалафил) Нарушения эрекции Таблетки 20 мг, №4</t>
   </si>
   <si>
@@ -124,13 +130,13 @@
     <t>Карнилев амп 1 г/5 мл №5 (левокарнитин)</t>
   </si>
   <si>
-    <t>04.23 МС 6 уп</t>
+    <t>04.23 МС</t>
   </si>
   <si>
     <t>Карнилев р-р 1г/10мл №10 (левокарнитин)</t>
   </si>
   <si>
-    <t>06.23 МС Аманат</t>
+    <t>06.23 МС и Аманат</t>
   </si>
   <si>
     <t>Лактоспей Беби саше№ 20 (Бифидобактерии BB-12, Стрептококк термофильный)</t>
@@ -170,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">Пантоспей таблетки 40 мг №28 (пантопразол) </t>
+  </si>
+  <si>
+    <t>09.23 МС</t>
   </si>
   <si>
     <t>Пантоспей фл. 40 мг №1 (пантопразол) пор. для приг. р-р для инъек</t>
@@ -642,6 +651,9 @@
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="3">
         <v>3500.0</v>
       </c>
@@ -649,7 +661,7 @@
         <v>44935.0</v>
       </c>
       <c r="F6" s="2">
-        <v>28.0</v>
+        <v>65.0</v>
       </c>
       <c r="M6" s="2">
         <v>29.0</v>
@@ -660,16 +672,22 @@
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="3">
         <v>7000.0</v>
       </c>
       <c r="F7" s="2">
-        <v>14.0</v>
+        <v>127.0</v>
       </c>
       <c r="H7" s="2">
-        <v>246.0</v>
+        <v>249.0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.0</v>
       </c>
       <c r="M7" s="2">
         <v>97.0</v>
@@ -680,13 +698,16 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2">
         <v>299.0</v>
       </c>
       <c r="F8" s="2">
-        <v>109.0</v>
+        <v>55.0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.0</v>
       </c>
       <c r="M8" s="2">
         <v>97.0</v>
@@ -697,19 +718,19 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D9" s="3">
         <v>10000.0</v>
       </c>
       <c r="F9" s="2">
-        <v>87.0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>5.0</v>
+        <v>295.0</v>
       </c>
       <c r="H9" s="2">
-        <v>44.0</v>
+        <v>45.0</v>
       </c>
       <c r="M9" s="2">
         <v>289.0</v>
@@ -720,7 +741,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3">
         <v>4500.0</v>
@@ -734,15 +755,18 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D11" s="3">
         <v>3500.0</v>
       </c>
       <c r="F11" s="2">
-        <v>16.0</v>
-      </c>
-      <c r="G11" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="K11" s="2">
         <v>1.0</v>
       </c>
       <c r="M11" s="2">
@@ -754,16 +778,13 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3">
         <v>1900.0</v>
       </c>
       <c r="F12" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>4.0</v>
+        <v>116.0</v>
       </c>
       <c r="M12" s="2">
         <v>306.0</v>
@@ -774,13 +795,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3">
         <v>2250.0</v>
       </c>
       <c r="F13" s="2">
-        <v>18.0</v>
+        <v>96.0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1.0</v>
       </c>
       <c r="M13" s="2">
         <v>100.0</v>
@@ -791,16 +815,22 @@
         <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3">
         <v>2180.0</v>
       </c>
       <c r="F14" s="2">
-        <v>181.0</v>
+        <v>405.0</v>
       </c>
       <c r="G14" s="2">
-        <v>55.0</v>
+        <v>127.0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.0</v>
       </c>
       <c r="M14" s="2">
         <v>218.0</v>
@@ -811,13 +841,22 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D15" s="3">
         <v>4800.0</v>
       </c>
       <c r="F15" s="2">
-        <v>3.0</v>
+        <v>110.0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.0</v>
       </c>
       <c r="M15" s="2">
         <v>61.0</v>
@@ -828,13 +867,19 @@
         <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D16" s="3">
         <v>7400.0</v>
       </c>
       <c r="F16" s="2">
-        <v>23.0</v>
+        <v>30.0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.0</v>
       </c>
       <c r="M16" s="2">
         <v>264.0</v>
@@ -845,17 +890,20 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3">
         <v>4150.0</v>
       </c>
       <c r="F17" s="2">
-        <v>55.0</v>
+        <v>98.0</v>
       </c>
       <c r="G17" s="2">
         <v>5.0</v>
       </c>
+      <c r="K17" s="2">
+        <v>1.0</v>
+      </c>
       <c r="M17" s="2">
         <v>62.0</v>
       </c>
@@ -865,13 +913,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D18" s="3">
         <v>6000.0</v>
       </c>
       <c r="F18" s="2">
-        <v>19.0</v>
+        <v>35.0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.0</v>
       </c>
       <c r="M18" s="2">
         <v>60.0</v>
@@ -882,7 +936,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D19" s="3">
         <v>7000.0</v>
@@ -893,11 +950,14 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" s="3">
         <v>1660.0</v>
       </c>
+      <c r="F20" s="2">
+        <v>59.0</v>
+      </c>
       <c r="M20" s="2">
         <v>97.0</v>
       </c>
@@ -907,7 +967,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D21" s="3">
         <v>35000.0</v>
@@ -918,13 +978,16 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2">
         <v>468.0</v>
       </c>
       <c r="F22" s="2">
-        <v>51.0</v>
+        <v>126.0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>16.0</v>
       </c>
       <c r="M22" s="2">
         <v>532.0</v>
@@ -935,16 +998,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D23" s="3">
         <v>2500.0</v>
       </c>
       <c r="F23" s="2">
-        <v>18.0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>5.0</v>
+        <v>25.0</v>
       </c>
       <c r="M23" s="2">
         <v>143.0</v>
@@ -955,22 +1015,28 @@
         <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D24" s="3">
         <v>4540.0</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2">
-        <v>47.0</v>
+        <v>8.0</v>
       </c>
       <c r="G24" s="2">
-        <v>28.0</v>
+        <v>20.0</v>
       </c>
       <c r="H24" s="2">
-        <v>113.0</v>
+        <v>114.0</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1.0</v>
       </c>
       <c r="M24" s="2">
         <v>110.0</v>
@@ -981,23 +1047,26 @@
         <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D25" s="3">
         <v>4258.0</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F25" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="G25" s="2">
-        <v>10.0</v>
+        <v>92.0</v>
       </c>
       <c r="H25" s="2">
         <v>174.0</v>
       </c>
+      <c r="K25" s="2">
+        <v>1.0</v>
+      </c>
       <c r="M25" s="2">
         <v>175.0</v>
       </c>
@@ -1007,19 +1076,19 @@
         <v>17</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D26" s="3">
         <v>3800.0</v>
       </c>
-      <c r="E26" s="1">
-        <v>44934.0</v>
-      </c>
       <c r="F26" s="2">
-        <v>29.0</v>
+        <v>54.0</v>
       </c>
       <c r="G26" s="2">
-        <v>8.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1.0</v>
       </c>
       <c r="M26" s="2">
         <v>96.0</v>
@@ -1030,16 +1099,16 @@
         <v>17</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D27" s="3">
         <v>4800.0</v>
       </c>
       <c r="F27" s="2">
-        <v>21.0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>5.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1.0</v>
       </c>
       <c r="M27" s="2">
         <v>174.0</v>
@@ -1050,16 +1119,16 @@
         <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D28" s="3">
         <v>4800.0</v>
       </c>
       <c r="F28" s="2">
-        <v>69.0</v>
+        <v>89.0</v>
       </c>
       <c r="G28" s="2">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="M28" s="2">
         <v>69.0</v>
@@ -1070,16 +1139,16 @@
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D29" s="3">
         <v>3100.0</v>
       </c>
       <c r="F29" s="2">
-        <v>36.0</v>
-      </c>
-      <c r="G29" s="2">
-        <v>6.0</v>
+        <v>26.0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1.0</v>
       </c>
       <c r="M29" s="2">
         <v>103.0</v>
@@ -1090,16 +1159,19 @@
         <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D30" s="3">
         <v>5000.0</v>
       </c>
       <c r="F30" s="2">
-        <v>37.0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>4.0</v>
+        <v>30.0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1.0</v>
       </c>
       <c r="M30" s="2">
         <v>148.0</v>
@@ -1110,16 +1182,22 @@
         <v>17</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D31" s="3">
         <v>4100.0</v>
       </c>
       <c r="F31" s="2">
-        <v>54.0</v>
+        <v>172.0</v>
       </c>
       <c r="H31" s="2">
-        <v>1003.0</v>
+        <v>1011.0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1.0</v>
       </c>
       <c r="M31" s="2">
         <v>706.0</v>
@@ -1130,7 +1208,10 @@
         <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D32" s="3">
         <v>3800.0</v>
@@ -1144,20 +1225,23 @@
         <v>17</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D33" s="3">
         <v>11000.0</v>
       </c>
       <c r="F33" s="2">
-        <v>35.0</v>
-      </c>
-      <c r="G33" s="2">
-        <v>3.0</v>
+        <v>43.0</v>
       </c>
       <c r="H33" s="2">
         <v>9.0</v>
       </c>
+      <c r="K33" s="2">
+        <v>1.0</v>
+      </c>
       <c r="M33" s="2">
         <v>213.0</v>
       </c>
@@ -1167,13 +1251,19 @@
         <v>17</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D34" s="3">
         <v>6300.0</v>
       </c>
       <c r="F34" s="2">
-        <v>79.0</v>
+        <v>26.0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1.0</v>
       </c>
       <c r="M34" s="2">
         <v>47.0</v>
@@ -1184,16 +1274,19 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D35" s="3">
         <v>4806.0</v>
       </c>
       <c r="F35" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="G35" s="2">
-        <v>18.0</v>
+        <v>129.0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1.0</v>
       </c>
       <c r="M35" s="2">
         <v>241.0</v>
@@ -1204,13 +1297,19 @@
         <v>17</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D36" s="3">
         <v>5800.0</v>
       </c>
       <c r="F36" s="2">
-        <v>16.0</v>
+        <v>225.0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1.0</v>
       </c>
       <c r="M36" s="2">
         <v>219.0</v>
@@ -1221,13 +1320,19 @@
         <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D37" s="3">
         <v>1950.0</v>
       </c>
       <c r="F37" s="2">
-        <v>30.0</v>
+        <v>95.0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1.0</v>
       </c>
       <c r="M37" s="2">
         <v>122.0</v>
@@ -1238,13 +1343,22 @@
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D38" s="3">
         <v>2650.0</v>
       </c>
+      <c r="E38" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="F38" s="2">
-        <v>8.0</v>
+        <v>258.0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1.0</v>
       </c>
       <c r="M38" s="2">
         <v>85.0</v>
@@ -1255,13 +1369,19 @@
         <v>17</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D39" s="3">
         <v>1700.0</v>
       </c>
-      <c r="G39" s="2">
-        <v>5.0</v>
+      <c r="F39" s="2">
+        <v>121.0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1.0</v>
       </c>
       <c r="M39" s="2">
         <v>329.0</v>
@@ -1272,11 +1392,20 @@
         <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D40" s="3">
         <v>8500.0</v>
       </c>
+      <c r="F40" s="2">
+        <v>91.0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1.0</v>
+      </c>
       <c r="M40" s="2">
         <v>297.0</v>
       </c>
@@ -1286,13 +1415,16 @@
         <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D41" s="3">
         <v>13000.0</v>
       </c>
       <c r="F41" s="2">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="M41" s="2">
         <v>28.0</v>
@@ -1303,7 +1435,10 @@
         <v>17</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D42" s="3">
         <v>9000.0</v>
@@ -1312,7 +1447,10 @@
         <v>44937.0</v>
       </c>
       <c r="F42" s="2">
-        <v>11.0</v>
+        <v>45.0</v>
+      </c>
+      <c r="K42" s="2">
+        <v>1.0</v>
       </c>
       <c r="M42" s="2">
         <v>19.0</v>
@@ -1323,16 +1461,19 @@
         <v>17</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D43" s="3">
         <v>4100.0</v>
       </c>
       <c r="F43" s="2">
-        <v>20.0</v>
+        <v>203.0</v>
       </c>
       <c r="H43" s="2">
-        <v>342.0</v>
+        <v>343.0</v>
       </c>
       <c r="M43" s="2">
         <v>199.0</v>
@@ -1343,16 +1484,19 @@
         <v>17</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D44" s="3">
         <v>8000.0</v>
       </c>
       <c r="F44" s="2">
-        <v>20.0</v>
+        <v>30.0</v>
       </c>
       <c r="G44" s="2">
-        <v>10.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1.0</v>
       </c>
       <c r="M44" s="2">
         <v>20.0</v>
@@ -1363,16 +1507,22 @@
         <v>17</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D45" s="3">
         <v>4000.0</v>
       </c>
       <c r="F45" s="2">
-        <v>21.0</v>
+        <v>87.0</v>
       </c>
       <c r="G45" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1.0</v>
       </c>
     </row>
     <row r="46">
@@ -1380,16 +1530,22 @@
         <v>17</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D46" s="3">
         <v>3200.0</v>
       </c>
       <c r="F46" s="2">
-        <v>145.0</v>
+        <v>67.0</v>
       </c>
       <c r="G46" s="2">
-        <v>15.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>1.0</v>
       </c>
       <c r="M46" s="2">
         <v>91.0</v>
@@ -1400,16 +1556,19 @@
         <v>17</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D47" s="3">
         <v>2300.0</v>
       </c>
       <c r="F47" s="2">
-        <v>34.0</v>
+        <v>49.0</v>
       </c>
       <c r="G47" s="2">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="M47" s="2">
         <v>205.0</v>
@@ -1420,16 +1579,16 @@
         <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D48" s="3">
         <v>3700.0</v>
       </c>
       <c r="F48" s="2">
-        <v>177.0</v>
-      </c>
-      <c r="G48" s="2">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="M48" s="2">
         <v>257.0</v>
@@ -1440,7 +1599,10 @@
         <v>17</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D49" s="3">
         <v>1500.0</v>
@@ -1449,7 +1611,7 @@
         <v>44932.0</v>
       </c>
       <c r="F49" s="2">
-        <v>50.0</v>
+        <v>266.0</v>
       </c>
       <c r="M49" s="2">
         <v>158.0</v>
@@ -1460,7 +1622,10 @@
         <v>17</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D50" s="3">
         <v>3500.0</v>
@@ -1469,7 +1634,7 @@
         <v>44932.0</v>
       </c>
       <c r="F50" s="2">
-        <v>102.0</v>
+        <v>42.0</v>
       </c>
       <c r="M50" s="2">
         <v>290.0</v>
@@ -1480,7 +1645,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D51" s="3">
         <v>30000.0</v>
@@ -1491,11 +1656,17 @@
         <v>17</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D52" s="3">
         <v>4500.0</v>
       </c>
+      <c r="F52" s="2">
+        <v>52.0</v>
+      </c>
       <c r="M52" s="2">
         <v>83.0</v>
       </c>
@@ -1505,13 +1676,25 @@
         <v>17</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D53" s="3">
         <v>1395.0</v>
       </c>
       <c r="F53" s="2">
-        <v>41.0</v>
+        <v>256.0</v>
+      </c>
+      <c r="G53" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K53" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="L53" s="2">
+        <v>3.0</v>
       </c>
       <c r="M53" s="2">
         <v>110.0</v>
@@ -1522,16 +1705,16 @@
         <v>17</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D54" s="3">
         <v>4800.0</v>
       </c>
       <c r="F54" s="2">
-        <v>55.0</v>
-      </c>
-      <c r="G54" s="2">
-        <v>11.0</v>
+        <v>80.0</v>
       </c>
       <c r="M54" s="2">
         <v>251.0</v>
@@ -1542,7 +1725,10 @@
         <v>17</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D55" s="3">
         <v>23900.0</v>
@@ -1551,7 +1737,10 @@
         <v>44934.0</v>
       </c>
       <c r="F55" s="2">
-        <v>31.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="K55" s="2">
+        <v>1.0</v>
       </c>
       <c r="M55" s="2">
         <v>18.0</v>
@@ -1562,7 +1751,10 @@
         <v>17</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D56" s="3">
         <v>20500.0</v>
@@ -1570,6 +1762,9 @@
       <c r="E56" s="1">
         <v>44932.0</v>
       </c>
+      <c r="K56" s="2">
+        <v>1.0</v>
+      </c>
       <c r="M56" s="2">
         <v>11.0</v>
       </c>
@@ -1579,16 +1774,16 @@
         <v>17</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D57" s="3">
         <v>15000.0</v>
       </c>
       <c r="F57" s="2">
-        <v>19.0</v>
-      </c>
-      <c r="G57" s="2">
-        <v>3.0</v>
+        <v>159.0</v>
+      </c>
+      <c r="K57" s="2">
+        <v>1.0</v>
       </c>
       <c r="M57" s="2">
         <v>128.0</v>
@@ -1599,16 +1794,22 @@
         <v>17</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D58" s="3">
         <v>2100.0</v>
       </c>
       <c r="F58" s="2">
-        <v>39.0</v>
+        <v>76.0</v>
       </c>
       <c r="G58" s="2">
-        <v>13.0</v>
+        <v>58.0</v>
+      </c>
+      <c r="K58" s="2">
+        <v>1.0</v>
       </c>
       <c r="M58" s="2">
         <v>265.0</v>
@@ -1619,16 +1820,22 @@
         <v>17</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D59" s="3">
         <v>10000.0</v>
       </c>
       <c r="F59" s="2">
-        <v>20.0</v>
+        <v>26.0</v>
       </c>
       <c r="G59" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="K59" s="2">
+        <v>1.0</v>
       </c>
       <c r="M59" s="2">
         <v>49.0</v>
@@ -1639,13 +1846,16 @@
         <v>17</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D60" s="3">
         <v>1735.0</v>
       </c>
       <c r="F60" s="2">
-        <v>31.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="K60" s="2">
+        <v>1.0</v>
       </c>
       <c r="M60" s="2">
         <v>120.0</v>
@@ -1656,7 +1866,7 @@
         <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D61" s="3">
         <v>2000.0</v>
@@ -1667,7 +1877,7 @@
         <v>17</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D62" s="3">
         <v>6000.0</v>
@@ -1684,19 +1894,19 @@
         <v>17</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D63" s="3">
         <v>3100.0</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F63" s="2">
-        <v>55.0</v>
-      </c>
-      <c r="G63" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="K63" s="2">
+        <v>1.0</v>
       </c>
       <c r="M63" s="2">
         <v>179.0</v>

</xml_diff>

<commit_message>
Optimising code in different files
</commit_message>
<xml_diff>
--- a/downloads/remains.xlsx
+++ b/downloads/remains.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Астана_Список_Остатков" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Караганда_Список_Остатков" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
   <si>
     <t>МСП</t>
   </si>
@@ -64,15 +64,12 @@
     <t>4/28/1905</t>
   </si>
   <si>
-    <t>Астана</t>
+    <t>Караганда</t>
   </si>
   <si>
     <t>Антикамен (почки) капс №60</t>
   </si>
   <si>
-    <t>М,К</t>
-  </si>
-  <si>
     <t>Беррилакт саше №30 (лактобактерии, манноза, экстр.клюквы)</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t xml:space="preserve">Бонеост (Ибандронат ) Таб покр пленоч оболоч 150 мг, №1  </t>
   </si>
   <si>
-    <t>Назгуль</t>
-  </si>
-  <si>
     <t>Волкрон (Тадалафил) Нарушения эрекции Таблетки 20 мг, №4</t>
   </si>
   <si>
@@ -130,13 +124,13 @@
     <t>Карнилев амп 1 г/5 мл №5 (левокарнитин)</t>
   </si>
   <si>
-    <t>04.23 МС</t>
+    <t>04.23 МС 6 уп</t>
   </si>
   <si>
     <t>Карнилев р-р 1г/10мл №10 (левокарнитин)</t>
   </si>
   <si>
-    <t>06.23 МС и Аманат</t>
+    <t>06.23 МС Аманат</t>
   </si>
   <si>
     <t>Лактоспей Беби саше№ 20 (Бифидобактерии BB-12, Стрептококк термофильный)</t>
@@ -176,9 +170,6 @@
   </si>
   <si>
     <t xml:space="preserve">Пантоспей таблетки 40 мг №28 (пантопразол) </t>
-  </si>
-  <si>
-    <t>09.23 МС</t>
   </si>
   <si>
     <t>Пантоспей фл. 40 мг №1 (пантопразол) пор. для приг. р-р для инъек</t>
@@ -651,9 +642,6 @@
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="3">
         <v>3500.0</v>
       </c>
@@ -661,7 +649,7 @@
         <v>44935.0</v>
       </c>
       <c r="F6" s="2">
-        <v>65.0</v>
+        <v>28.0</v>
       </c>
       <c r="M6" s="2">
         <v>29.0</v>
@@ -672,22 +660,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="3">
         <v>7000.0</v>
       </c>
       <c r="F7" s="2">
-        <v>127.0</v>
+        <v>14.0</v>
       </c>
       <c r="H7" s="2">
-        <v>249.0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1.0</v>
+        <v>246.0</v>
       </c>
       <c r="M7" s="2">
         <v>97.0</v>
@@ -698,16 +680,13 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2">
         <v>299.0</v>
       </c>
       <c r="F8" s="2">
-        <v>55.0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1.0</v>
+        <v>109.0</v>
       </c>
       <c r="M8" s="2">
         <v>97.0</v>
@@ -718,19 +697,19 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3">
         <v>10000.0</v>
       </c>
       <c r="F9" s="2">
-        <v>295.0</v>
+        <v>87.0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5.0</v>
       </c>
       <c r="H9" s="2">
-        <v>45.0</v>
+        <v>44.0</v>
       </c>
       <c r="M9" s="2">
         <v>289.0</v>
@@ -741,7 +720,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="3">
         <v>4500.0</v>
@@ -755,18 +734,15 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3">
         <v>3500.0</v>
       </c>
       <c r="F11" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="K11" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="G11" s="2">
         <v>1.0</v>
       </c>
       <c r="M11" s="2">
@@ -778,13 +754,16 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3">
         <v>1900.0</v>
       </c>
       <c r="F12" s="2">
-        <v>116.0</v>
+        <v>50.0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4.0</v>
       </c>
       <c r="M12" s="2">
         <v>306.0</v>
@@ -795,16 +774,13 @@
         <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="3">
         <v>2250.0</v>
       </c>
       <c r="F13" s="2">
-        <v>96.0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1.0</v>
+        <v>18.0</v>
       </c>
       <c r="M13" s="2">
         <v>100.0</v>
@@ -815,22 +791,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3">
         <v>2180.0</v>
       </c>
       <c r="F14" s="2">
-        <v>405.0</v>
+        <v>181.0</v>
       </c>
       <c r="G14" s="2">
-        <v>127.0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1.0</v>
+        <v>55.0</v>
       </c>
       <c r="M14" s="2">
         <v>218.0</v>
@@ -841,22 +811,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3">
         <v>4800.0</v>
       </c>
       <c r="F15" s="2">
-        <v>110.0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>9.0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="M15" s="2">
         <v>61.0</v>
@@ -867,19 +828,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D16" s="3">
         <v>7400.0</v>
       </c>
       <c r="F16" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1.0</v>
+        <v>23.0</v>
       </c>
       <c r="M16" s="2">
         <v>264.0</v>
@@ -890,20 +845,17 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3">
         <v>4150.0</v>
       </c>
       <c r="F17" s="2">
-        <v>98.0</v>
+        <v>55.0</v>
       </c>
       <c r="G17" s="2">
         <v>5.0</v>
       </c>
-      <c r="K17" s="2">
-        <v>1.0</v>
-      </c>
       <c r="M17" s="2">
         <v>62.0</v>
       </c>
@@ -913,19 +865,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D18" s="3">
         <v>6000.0</v>
       </c>
       <c r="F18" s="2">
-        <v>35.0</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1.0</v>
+        <v>19.0</v>
       </c>
       <c r="M18" s="2">
         <v>60.0</v>
@@ -936,10 +882,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3">
         <v>7000.0</v>
@@ -950,14 +893,11 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="3">
         <v>1660.0</v>
       </c>
-      <c r="F20" s="2">
-        <v>59.0</v>
-      </c>
       <c r="M20" s="2">
         <v>97.0</v>
       </c>
@@ -967,7 +907,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D21" s="3">
         <v>35000.0</v>
@@ -978,16 +918,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2">
         <v>468.0</v>
       </c>
       <c r="F22" s="2">
-        <v>126.0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>16.0</v>
+        <v>51.0</v>
       </c>
       <c r="M22" s="2">
         <v>532.0</v>
@@ -998,13 +935,16 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D23" s="3">
         <v>2500.0</v>
       </c>
       <c r="F23" s="2">
-        <v>25.0</v>
+        <v>18.0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5.0</v>
       </c>
       <c r="M23" s="2">
         <v>143.0</v>
@@ -1015,28 +955,22 @@
         <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D24" s="3">
         <v>4540.0</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F24" s="2">
-        <v>8.0</v>
+        <v>47.0</v>
       </c>
       <c r="G24" s="2">
-        <v>20.0</v>
+        <v>28.0</v>
       </c>
       <c r="H24" s="2">
-        <v>114.0</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1.0</v>
+        <v>113.0</v>
       </c>
       <c r="M24" s="2">
         <v>110.0</v>
@@ -1047,26 +981,23 @@
         <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D25" s="3">
         <v>4258.0</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2">
-        <v>92.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>10.0</v>
       </c>
       <c r="H25" s="2">
         <v>174.0</v>
       </c>
-      <c r="K25" s="2">
-        <v>1.0</v>
-      </c>
       <c r="M25" s="2">
         <v>175.0</v>
       </c>
@@ -1076,19 +1007,19 @@
         <v>17</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="3">
         <v>3800.0</v>
       </c>
+      <c r="E26" s="1">
+        <v>44934.0</v>
+      </c>
       <c r="F26" s="2">
-        <v>54.0</v>
+        <v>29.0</v>
       </c>
       <c r="G26" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="M26" s="2">
         <v>96.0</v>
@@ -1099,16 +1030,16 @@
         <v>17</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="3">
         <v>4800.0</v>
       </c>
       <c r="F27" s="2">
-        <v>39.0</v>
-      </c>
-      <c r="K27" s="2">
-        <v>1.0</v>
+        <v>21.0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>5.0</v>
       </c>
       <c r="M27" s="2">
         <v>174.0</v>
@@ -1119,16 +1050,16 @@
         <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="3">
         <v>4800.0</v>
       </c>
       <c r="F28" s="2">
-        <v>89.0</v>
+        <v>69.0</v>
       </c>
       <c r="G28" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="M28" s="2">
         <v>69.0</v>
@@ -1139,16 +1070,16 @@
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D29" s="3">
         <v>3100.0</v>
       </c>
       <c r="F29" s="2">
-        <v>26.0</v>
-      </c>
-      <c r="K29" s="2">
-        <v>1.0</v>
+        <v>36.0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>6.0</v>
       </c>
       <c r="M29" s="2">
         <v>103.0</v>
@@ -1159,19 +1090,16 @@
         <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D30" s="3">
         <v>5000.0</v>
       </c>
       <c r="F30" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="K30" s="2">
-        <v>1.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4.0</v>
       </c>
       <c r="M30" s="2">
         <v>148.0</v>
@@ -1182,22 +1110,16 @@
         <v>17</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D31" s="3">
         <v>4100.0</v>
       </c>
       <c r="F31" s="2">
-        <v>172.0</v>
+        <v>54.0</v>
       </c>
       <c r="H31" s="2">
-        <v>1011.0</v>
-      </c>
-      <c r="I31" s="2">
-        <v>1.0</v>
+        <v>1003.0</v>
       </c>
       <c r="M31" s="2">
         <v>706.0</v>
@@ -1208,10 +1130,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D32" s="3">
         <v>3800.0</v>
@@ -1225,23 +1144,20 @@
         <v>17</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D33" s="3">
         <v>11000.0</v>
       </c>
       <c r="F33" s="2">
-        <v>43.0</v>
+        <v>35.0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>3.0</v>
       </c>
       <c r="H33" s="2">
         <v>9.0</v>
       </c>
-      <c r="K33" s="2">
-        <v>1.0</v>
-      </c>
       <c r="M33" s="2">
         <v>213.0</v>
       </c>
@@ -1251,19 +1167,13 @@
         <v>17</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3">
         <v>6300.0</v>
       </c>
       <c r="F34" s="2">
-        <v>26.0</v>
-      </c>
-      <c r="K34" s="2">
-        <v>1.0</v>
+        <v>79.0</v>
       </c>
       <c r="M34" s="2">
         <v>47.0</v>
@@ -1274,19 +1184,16 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D35" s="3">
         <v>4806.0</v>
       </c>
       <c r="F35" s="2">
-        <v>129.0</v>
-      </c>
-      <c r="K35" s="2">
-        <v>1.0</v>
+        <v>80.0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>18.0</v>
       </c>
       <c r="M35" s="2">
         <v>241.0</v>
@@ -1297,19 +1204,13 @@
         <v>17</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D36" s="3">
         <v>5800.0</v>
       </c>
       <c r="F36" s="2">
-        <v>225.0</v>
-      </c>
-      <c r="K36" s="2">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
       <c r="M36" s="2">
         <v>219.0</v>
@@ -1320,19 +1221,13 @@
         <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D37" s="3">
         <v>1950.0</v>
       </c>
       <c r="F37" s="2">
-        <v>95.0</v>
-      </c>
-      <c r="K37" s="2">
-        <v>1.0</v>
+        <v>30.0</v>
       </c>
       <c r="M37" s="2">
         <v>122.0</v>
@@ -1343,22 +1238,13 @@
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D38" s="3">
         <v>2650.0</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F38" s="2">
-        <v>258.0</v>
-      </c>
-      <c r="K38" s="2">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="M38" s="2">
         <v>85.0</v>
@@ -1369,19 +1255,13 @@
         <v>17</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D39" s="3">
         <v>1700.0</v>
       </c>
-      <c r="F39" s="2">
-        <v>121.0</v>
-      </c>
-      <c r="K39" s="2">
-        <v>1.0</v>
+      <c r="G39" s="2">
+        <v>5.0</v>
       </c>
       <c r="M39" s="2">
         <v>329.0</v>
@@ -1392,20 +1272,11 @@
         <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="D40" s="3">
         <v>8500.0</v>
       </c>
-      <c r="F40" s="2">
-        <v>91.0</v>
-      </c>
-      <c r="K40" s="2">
-        <v>1.0</v>
-      </c>
       <c r="M40" s="2">
         <v>297.0</v>
       </c>
@@ -1415,16 +1286,13 @@
         <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D41" s="3">
         <v>13000.0</v>
       </c>
       <c r="F41" s="2">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="M41" s="2">
         <v>28.0</v>
@@ -1435,10 +1303,7 @@
         <v>17</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D42" s="3">
         <v>9000.0</v>
@@ -1447,10 +1312,7 @@
         <v>44937.0</v>
       </c>
       <c r="F42" s="2">
-        <v>45.0</v>
-      </c>
-      <c r="K42" s="2">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="M42" s="2">
         <v>19.0</v>
@@ -1461,19 +1323,16 @@
         <v>17</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D43" s="3">
         <v>4100.0</v>
       </c>
       <c r="F43" s="2">
-        <v>203.0</v>
+        <v>20.0</v>
       </c>
       <c r="H43" s="2">
-        <v>343.0</v>
+        <v>342.0</v>
       </c>
       <c r="M43" s="2">
         <v>199.0</v>
@@ -1484,19 +1343,16 @@
         <v>17</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D44" s="3">
         <v>8000.0</v>
       </c>
       <c r="F44" s="2">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="G44" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K44" s="2">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="M44" s="2">
         <v>20.0</v>
@@ -1507,22 +1363,16 @@
         <v>17</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D45" s="3">
         <v>4000.0</v>
       </c>
       <c r="F45" s="2">
-        <v>87.0</v>
+        <v>21.0</v>
       </c>
       <c r="G45" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="K45" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="46">
@@ -1530,22 +1380,16 @@
         <v>17</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D46" s="3">
         <v>3200.0</v>
       </c>
       <c r="F46" s="2">
-        <v>67.0</v>
+        <v>145.0</v>
       </c>
       <c r="G46" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K46" s="2">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="M46" s="2">
         <v>91.0</v>
@@ -1556,19 +1400,16 @@
         <v>17</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="D47" s="3">
         <v>2300.0</v>
       </c>
       <c r="F47" s="2">
-        <v>49.0</v>
+        <v>34.0</v>
       </c>
       <c r="G47" s="2">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="M47" s="2">
         <v>205.0</v>
@@ -1579,16 +1420,16 @@
         <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D48" s="3">
         <v>3700.0</v>
       </c>
       <c r="F48" s="2">
-        <v>21.0</v>
+        <v>177.0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>3.0</v>
       </c>
       <c r="M48" s="2">
         <v>257.0</v>
@@ -1599,10 +1440,7 @@
         <v>17</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D49" s="3">
         <v>1500.0</v>
@@ -1611,7 +1449,7 @@
         <v>44932.0</v>
       </c>
       <c r="F49" s="2">
-        <v>266.0</v>
+        <v>50.0</v>
       </c>
       <c r="M49" s="2">
         <v>158.0</v>
@@ -1622,10 +1460,7 @@
         <v>17</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="D50" s="3">
         <v>3500.0</v>
@@ -1634,7 +1469,7 @@
         <v>44932.0</v>
       </c>
       <c r="F50" s="2">
-        <v>42.0</v>
+        <v>102.0</v>
       </c>
       <c r="M50" s="2">
         <v>290.0</v>
@@ -1645,7 +1480,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D51" s="3">
         <v>30000.0</v>
@@ -1656,17 +1491,11 @@
         <v>17</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="D52" s="3">
         <v>4500.0</v>
       </c>
-      <c r="F52" s="2">
-        <v>52.0</v>
-      </c>
       <c r="M52" s="2">
         <v>83.0</v>
       </c>
@@ -1676,25 +1505,13 @@
         <v>17</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="D53" s="3">
         <v>1395.0</v>
       </c>
       <c r="F53" s="2">
-        <v>256.0</v>
-      </c>
-      <c r="G53" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K53" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="L53" s="2">
-        <v>3.0</v>
+        <v>41.0</v>
       </c>
       <c r="M53" s="2">
         <v>110.0</v>
@@ -1705,16 +1522,16 @@
         <v>17</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D54" s="3">
         <v>4800.0</v>
       </c>
       <c r="F54" s="2">
-        <v>80.0</v>
+        <v>55.0</v>
+      </c>
+      <c r="G54" s="2">
+        <v>11.0</v>
       </c>
       <c r="M54" s="2">
         <v>251.0</v>
@@ -1725,10 +1542,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D55" s="3">
         <v>23900.0</v>
@@ -1737,10 +1551,7 @@
         <v>44934.0</v>
       </c>
       <c r="F55" s="2">
-        <v>42.0</v>
-      </c>
-      <c r="K55" s="2">
-        <v>1.0</v>
+        <v>31.0</v>
       </c>
       <c r="M55" s="2">
         <v>18.0</v>
@@ -1751,10 +1562,7 @@
         <v>17</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D56" s="3">
         <v>20500.0</v>
@@ -1762,9 +1570,6 @@
       <c r="E56" s="1">
         <v>44932.0</v>
       </c>
-      <c r="K56" s="2">
-        <v>1.0</v>
-      </c>
       <c r="M56" s="2">
         <v>11.0</v>
       </c>
@@ -1774,16 +1579,16 @@
         <v>17</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D57" s="3">
         <v>15000.0</v>
       </c>
       <c r="F57" s="2">
-        <v>159.0</v>
-      </c>
-      <c r="K57" s="2">
-        <v>1.0</v>
+        <v>19.0</v>
+      </c>
+      <c r="G57" s="2">
+        <v>3.0</v>
       </c>
       <c r="M57" s="2">
         <v>128.0</v>
@@ -1794,22 +1599,16 @@
         <v>17</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="D58" s="3">
         <v>2100.0</v>
       </c>
       <c r="F58" s="2">
-        <v>76.0</v>
+        <v>39.0</v>
       </c>
       <c r="G58" s="2">
-        <v>58.0</v>
-      </c>
-      <c r="K58" s="2">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="M58" s="2">
         <v>265.0</v>
@@ -1820,22 +1619,16 @@
         <v>17</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="D59" s="3">
         <v>10000.0</v>
       </c>
       <c r="F59" s="2">
-        <v>26.0</v>
+        <v>20.0</v>
       </c>
       <c r="G59" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K59" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="M59" s="2">
         <v>49.0</v>
@@ -1846,16 +1639,13 @@
         <v>17</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D60" s="3">
         <v>1735.0</v>
       </c>
       <c r="F60" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K60" s="2">
-        <v>1.0</v>
+        <v>31.0</v>
       </c>
       <c r="M60" s="2">
         <v>120.0</v>
@@ -1866,7 +1656,7 @@
         <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D61" s="3">
         <v>2000.0</v>
@@ -1877,7 +1667,7 @@
         <v>17</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D62" s="3">
         <v>6000.0</v>
@@ -1894,19 +1684,19 @@
         <v>17</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D63" s="3">
         <v>3100.0</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F63" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K63" s="2">
-        <v>1.0</v>
+        <v>55.0</v>
+      </c>
+      <c r="G63" s="2">
+        <v>2.0</v>
       </c>
       <c r="M63" s="2">
         <v>179.0</v>

</xml_diff>